<commit_message>
Clean-up the build process
</commit_message>
<xml_diff>
--- a/files/2019-2020/Zaalschema 2019-2020 v2.xlsx
+++ b/files/2019-2020/Zaalschema 2019-2020 v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwin/Projects/zod-zaalvoetbal/files/2019-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA983CC-772E-5845-B764-5A1783E6741D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0C318C-50FD-0344-8D47-F006868289F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="32800" windowHeight="20540" tabRatio="833" firstSheet="10" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="4200" windowWidth="20660" windowHeight="16800" tabRatio="833" firstSheet="13" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O13-A" sheetId="85" r:id="rId1"/>
@@ -1495,42 +1495,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1603,7 +1567,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1952,7 +1952,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8806,7 +8806,7 @@
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B2" s="302" t="s">
+      <c r="B2" s="290" t="s">
         <v>235</v>
       </c>
       <c r="C2">
@@ -8814,11 +8814,11 @@
       </c>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
-      <c r="N2" s="301"/>
+      <c r="N2" s="289"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B3" s="303" t="s">
+      <c r="B3" s="291" t="s">
         <v>237</v>
       </c>
       <c r="C3">
@@ -8826,7 +8826,7 @@
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
-      <c r="N3" s="301"/>
+      <c r="N3" s="289"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -8839,11 +8839,11 @@
       <c r="F4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="301"/>
+      <c r="N4" s="289"/>
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="306" t="s">
+      <c r="B5" s="294" t="s">
         <v>239</v>
       </c>
       <c r="C5">
@@ -8851,7 +8851,7 @@
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="301"/>
+      <c r="N5" s="289"/>
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
@@ -8863,11 +8863,11 @@
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="301"/>
+      <c r="N6" s="289"/>
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B7" s="304" t="s">
+      <c r="B7" s="292" t="s">
         <v>240</v>
       </c>
       <c r="C7">
@@ -8875,11 +8875,11 @@
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="301"/>
+      <c r="N7" s="289"/>
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B8" s="305" t="s">
+      <c r="B8" s="293" t="s">
         <v>241</v>
       </c>
       <c r="C8" s="9">
@@ -8887,7 +8887,7 @@
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="301"/>
+      <c r="N8" s="289"/>
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
@@ -8897,28 +8897,28 @@
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="301"/>
+      <c r="N9" s="289"/>
       <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="280">
         <v>43820</v>
       </c>
-      <c r="B10" s="343" t="s">
+      <c r="B10" s="331" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="343"/>
-      <c r="D10" s="344"/>
-      <c r="E10" s="344"/>
+      <c r="C10" s="331"/>
+      <c r="D10" s="332"/>
+      <c r="E10" s="332"/>
       <c r="F10" s="280">
         <v>43820</v>
       </c>
-      <c r="G10" s="343" t="s">
+      <c r="G10" s="331" t="s">
         <v>189</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="301"/>
+      <c r="N10" s="289"/>
       <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
@@ -8930,202 +8930,202 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="307" t="s">
+      <c r="A12" s="295" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="307" t="s">
+      <c r="B12" s="295" t="s">
         <v>193</v>
       </c>
-      <c r="C12" s="308" t="s">
+      <c r="C12" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="D12" s="309" t="s">
+      <c r="D12" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="E12" s="310"/>
-      <c r="F12" s="307" t="s">
+      <c r="E12" s="298"/>
+      <c r="F12" s="295" t="s">
         <v>192</v>
       </c>
-      <c r="G12" s="307" t="s">
+      <c r="G12" s="295" t="s">
         <v>193</v>
       </c>
-      <c r="H12" s="311" t="s">
+      <c r="H12" s="299" t="s">
         <v>238</v>
       </c>
-      <c r="I12" s="312" t="s">
+      <c r="I12" s="300" t="s">
         <v>236</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" s="307" t="s">
+      <c r="A13" s="295" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="307" t="s">
+      <c r="B13" s="295" t="s">
         <v>195</v>
       </c>
-      <c r="C13" s="309" t="s">
+      <c r="C13" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="D13" s="311" t="s">
+      <c r="D13" s="299" t="s">
         <v>238</v>
       </c>
-      <c r="E13" s="310"/>
-      <c r="F13" s="307" t="s">
+      <c r="E13" s="298"/>
+      <c r="F13" s="295" t="s">
         <v>194</v>
       </c>
-      <c r="G13" s="307" t="s">
+      <c r="G13" s="295" t="s">
         <v>195</v>
       </c>
-      <c r="H13" s="313" t="s">
+      <c r="H13" s="301" t="s">
         <v>240</v>
       </c>
-      <c r="I13" s="314" t="s">
+      <c r="I13" s="302" t="s">
         <v>241</v>
       </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="301"/>
+      <c r="N13" s="289"/>
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A14" s="307" t="s">
+      <c r="A14" s="295" t="s">
         <v>196</v>
       </c>
-      <c r="B14" s="307" t="s">
+      <c r="B14" s="295" t="s">
         <v>197</v>
       </c>
-      <c r="C14" s="312" t="s">
+      <c r="C14" s="300" t="s">
         <v>236</v>
       </c>
-      <c r="D14" s="314" t="s">
+      <c r="D14" s="302" t="s">
         <v>241</v>
       </c>
-      <c r="E14" s="310"/>
-      <c r="F14" s="307" t="s">
+      <c r="E14" s="298"/>
+      <c r="F14" s="295" t="s">
         <v>196</v>
       </c>
-      <c r="G14" s="307" t="s">
+      <c r="G14" s="295" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="308" t="s">
+      <c r="H14" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="I14" s="315" t="s">
+      <c r="I14" s="303" t="s">
         <v>239</v>
       </c>
       <c r="J14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="301"/>
+      <c r="N14" s="289"/>
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" s="307" t="s">
+      <c r="A15" s="295" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="307" t="s">
+      <c r="B15" s="295" t="s">
         <v>199</v>
       </c>
-      <c r="C15" s="312" t="s">
+      <c r="C15" s="300" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="313" t="s">
+      <c r="D15" s="301" t="s">
         <v>240</v>
       </c>
-      <c r="E15" s="310"/>
-      <c r="F15" s="307" t="s">
+      <c r="E15" s="298"/>
+      <c r="F15" s="295" t="s">
         <v>198</v>
       </c>
-      <c r="G15" s="307" t="s">
+      <c r="G15" s="295" t="s">
         <v>199</v>
       </c>
-      <c r="H15" s="311" t="s">
+      <c r="H15" s="299" t="s">
         <v>238</v>
       </c>
-      <c r="I15" s="315" t="s">
+      <c r="I15" s="303" t="s">
         <v>239</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="301"/>
+      <c r="N15" s="289"/>
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A16" s="307" t="s">
+      <c r="A16" s="295" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="307" t="s">
+      <c r="B16" s="295" t="s">
         <v>201</v>
       </c>
-      <c r="C16" s="314" t="s">
+      <c r="C16" s="302" t="s">
         <v>241</v>
       </c>
-      <c r="D16" s="308" t="s">
+      <c r="D16" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="310"/>
-      <c r="F16" s="307" t="s">
+      <c r="E16" s="298"/>
+      <c r="F16" s="295" t="s">
         <v>200</v>
       </c>
-      <c r="G16" s="307" t="s">
+      <c r="G16" s="295" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="309" t="s">
+      <c r="H16" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="I16" s="313" t="s">
+      <c r="I16" s="301" t="s">
         <v>240</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="301"/>
+      <c r="N16" s="289"/>
       <c r="O16" s="9"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="301"/>
+      <c r="N17" s="289"/>
       <c r="O17" s="9"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A19" s="340">
+      <c r="A19" s="328">
         <v>43841</v>
       </c>
-      <c r="B19" s="341" t="s">
+      <c r="B19" s="329" t="s">
         <v>242</v>
       </c>
-      <c r="C19" s="342"/>
-      <c r="D19" s="342"/>
-      <c r="E19" s="342"/>
-      <c r="F19" s="340">
+      <c r="C19" s="330"/>
+      <c r="D19" s="330"/>
+      <c r="E19" s="330"/>
+      <c r="F19" s="328">
         <v>43841</v>
       </c>
-      <c r="G19" s="341" t="s">
+      <c r="G19" s="329" t="s">
         <v>242</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A20" s="336"/>
-      <c r="B20" s="337"/>
+      <c r="A20" s="324"/>
+      <c r="B20" s="325"/>
       <c r="C20" s="11" t="s">
         <v>190</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="336"/>
-      <c r="G20" s="337"/>
+      <c r="F20" s="324"/>
+      <c r="G20" s="325"/>
       <c r="H20" s="9" t="s">
         <v>191</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="301"/>
+      <c r="N20" s="289"/>
       <c r="O20" s="9"/>
       <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
@@ -9133,35 +9133,35 @@
       <c r="T20" s="9"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A21" s="307" t="s">
+      <c r="A21" s="295" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="307" t="s">
+      <c r="B21" s="295" t="s">
         <v>193</v>
       </c>
-      <c r="C21" s="309" t="s">
+      <c r="C21" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="D21" s="315" t="s">
+      <c r="D21" s="303" t="s">
         <v>239</v>
       </c>
-      <c r="E21" s="310"/>
-      <c r="F21" s="307" t="s">
+      <c r="E21" s="298"/>
+      <c r="F21" s="295" t="s">
         <v>192</v>
       </c>
-      <c r="G21" s="307" t="s">
+      <c r="G21" s="295" t="s">
         <v>193</v>
       </c>
-      <c r="H21" s="308" t="s">
+      <c r="H21" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="I21" s="311" t="s">
+      <c r="I21" s="299" t="s">
         <v>238</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="301"/>
+      <c r="N21" s="289"/>
       <c r="O21" s="9"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
@@ -9169,63 +9169,63 @@
       <c r="T21" s="9"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A22" s="307" t="s">
+      <c r="A22" s="295" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="307" t="s">
+      <c r="B22" s="295" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="311" t="s">
+      <c r="C22" s="299" t="s">
         <v>238</v>
       </c>
-      <c r="D22" s="313" t="s">
+      <c r="D22" s="301" t="s">
         <v>240</v>
       </c>
-      <c r="E22" s="310"/>
-      <c r="F22" s="307" t="s">
+      <c r="E22" s="298"/>
+      <c r="F22" s="295" t="s">
         <v>194</v>
       </c>
-      <c r="G22" s="307" t="s">
+      <c r="G22" s="295" t="s">
         <v>195</v>
       </c>
-      <c r="H22" s="315" t="s">
+      <c r="H22" s="303" t="s">
         <v>239</v>
       </c>
-      <c r="I22" s="312" t="s">
+      <c r="I22" s="300" t="s">
         <v>236</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="301"/>
+      <c r="N22" s="289"/>
       <c r="O22" s="9"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A23" s="307" t="s">
+      <c r="A23" s="295" t="s">
         <v>196</v>
       </c>
-      <c r="B23" s="307" t="s">
+      <c r="B23" s="295" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="314" t="s">
+      <c r="C23" s="302" t="s">
         <v>241</v>
       </c>
-      <c r="D23" s="309" t="s">
+      <c r="D23" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="E23" s="310"/>
-      <c r="F23" s="307" t="s">
+      <c r="E23" s="298"/>
+      <c r="F23" s="295" t="s">
         <v>196</v>
       </c>
-      <c r="G23" s="307" t="s">
+      <c r="G23" s="295" t="s">
         <v>197</v>
       </c>
-      <c r="H23" s="339"/>
-      <c r="I23" s="339"/>
+      <c r="H23" s="327"/>
+      <c r="I23" s="327"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="301"/>
+      <c r="N23" s="289"/>
       <c r="O23" s="9"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
@@ -9233,29 +9233,29 @@
       <c r="T23" s="9"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A24" s="307" t="s">
+      <c r="A24" s="295" t="s">
         <v>198</v>
       </c>
-      <c r="B24" s="307" t="s">
+      <c r="B24" s="295" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="313" t="s">
+      <c r="C24" s="301" t="s">
         <v>240</v>
       </c>
-      <c r="D24" s="315" t="s">
+      <c r="D24" s="303" t="s">
         <v>239</v>
       </c>
-      <c r="E24" s="310"/>
-      <c r="F24" s="307" t="s">
+      <c r="E24" s="298"/>
+      <c r="F24" s="295" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="307" t="s">
+      <c r="G24" s="295" t="s">
         <v>199</v>
       </c>
-      <c r="H24" s="311" t="s">
+      <c r="H24" s="299" t="s">
         <v>238</v>
       </c>
-      <c r="I24" s="314" t="s">
+      <c r="I24" s="302" t="s">
         <v>241</v>
       </c>
       <c r="L24" s="9"/>
@@ -9266,34 +9266,34 @@
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A25" s="307" t="s">
+      <c r="A25" s="295" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="307" t="s">
+      <c r="B25" s="295" t="s">
         <v>201</v>
       </c>
-      <c r="C25" s="312" t="s">
+      <c r="C25" s="300" t="s">
         <v>236</v>
       </c>
-      <c r="D25" s="308" t="s">
+      <c r="D25" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="E25" s="310"/>
-      <c r="F25" s="307" t="s">
+      <c r="E25" s="298"/>
+      <c r="F25" s="295" t="s">
         <v>200</v>
       </c>
-      <c r="G25" s="307" t="s">
+      <c r="G25" s="295" t="s">
         <v>201</v>
       </c>
-      <c r="H25" s="309" t="s">
+      <c r="H25" s="297" t="s">
         <v>237</v>
       </c>
-      <c r="I25" s="312" t="s">
+      <c r="I25" s="300" t="s">
         <v>236</v>
       </c>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
-      <c r="N25" s="301"/>
+      <c r="N25" s="289"/>
       <c r="O25" s="9"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
@@ -9301,50 +9301,50 @@
       <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A26" s="307" t="s">
+      <c r="A26" s="295" t="s">
         <v>202</v>
       </c>
-      <c r="B26" s="307" t="s">
+      <c r="B26" s="295" t="s">
         <v>203</v>
       </c>
-      <c r="C26" s="308" t="s">
+      <c r="C26" s="296" t="s">
         <v>235</v>
       </c>
-      <c r="D26" s="313" t="s">
+      <c r="D26" s="301" t="s">
         <v>240</v>
       </c>
-      <c r="E26" s="310"/>
-      <c r="F26" s="307" t="s">
+      <c r="E26" s="298"/>
+      <c r="F26" s="295" t="s">
         <v>202</v>
       </c>
-      <c r="G26" s="307" t="s">
+      <c r="G26" s="295" t="s">
         <v>203</v>
       </c>
-      <c r="H26" s="315" t="s">
+      <c r="H26" s="303" t="s">
         <v>239</v>
       </c>
-      <c r="I26" s="314" t="s">
+      <c r="I26" s="302" t="s">
         <v>241</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
-      <c r="N26" s="301"/>
+      <c r="N26" s="289"/>
       <c r="O26" s="9"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A27" s="317"/>
-      <c r="B27" s="317"/>
+      <c r="A27" s="305"/>
+      <c r="B27" s="305"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
-      <c r="N27" s="301"/>
+      <c r="N27" s="289"/>
       <c r="O27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A28" s="317"/>
-      <c r="B28" s="317" t="s">
+      <c r="A28" s="305"/>
+      <c r="B28" s="305" t="s">
         <v>204</v>
       </c>
-      <c r="C28" s="338">
+      <c r="C28" s="326">
         <v>43476</v>
       </c>
       <c r="L28" s="9"/>
@@ -9375,7 +9375,7 @@
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
-      <c r="N30" s="301"/>
+      <c r="N30" s="289"/>
       <c r="O30" s="9"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
@@ -9390,7 +9390,7 @@
       </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="301"/>
+      <c r="N31" s="289"/>
       <c r="O31" s="9"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.15">
@@ -9422,7 +9422,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="301"/>
+      <c r="K33" s="289"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
@@ -9435,13 +9435,13 @@
         <v>3</v>
       </c>
       <c r="D34" s="9"/>
-      <c r="E34" s="301"/>
-      <c r="F34" s="301"/>
-      <c r="I34" s="301"/>
-      <c r="J34" s="301"/>
+      <c r="E34" s="289"/>
+      <c r="F34" s="289"/>
+      <c r="I34" s="289"/>
+      <c r="J34" s="289"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
-      <c r="N34" s="301"/>
+      <c r="N34" s="289"/>
       <c r="O34" s="9"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
@@ -9454,18 +9454,18 @@
       <c r="C35" s="1">
         <v>3</v>
       </c>
-      <c r="D35" s="301"/>
-      <c r="E35" s="301"/>
-      <c r="F35" s="301"/>
-      <c r="G35" s="301"/>
-      <c r="J35" s="301"/>
+      <c r="D35" s="289"/>
+      <c r="E35" s="289"/>
+      <c r="F35" s="289"/>
+      <c r="G35" s="289"/>
+      <c r="J35" s="289"/>
       <c r="L35" s="9"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
-      <c r="B36" s="338"/>
-      <c r="C36" s="338"/>
-      <c r="D36" s="301"/>
+      <c r="B36" s="326"/>
+      <c r="C36" s="326"/>
+      <c r="D36" s="289"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="9"/>
@@ -9475,11 +9475,11 @@
       <c r="C37" s="1">
         <v>22</v>
       </c>
-      <c r="E37" s="301"/>
-      <c r="F37" s="301"/>
-      <c r="H37" s="301"/>
-      <c r="I37" s="301"/>
-      <c r="J37" s="301"/>
+      <c r="E37" s="289"/>
+      <c r="F37" s="289"/>
+      <c r="H37" s="289"/>
+      <c r="I37" s="289"/>
+      <c r="J37" s="289"/>
       <c r="M37" s="9"/>
     </row>
   </sheetData>
@@ -9494,9 +9494,9 @@
   </sheetPr>
   <dimension ref="A1:AW258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="165" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M243" sqref="M243"/>
+      <selection pane="topRight" activeCell="E233" sqref="E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9536,66 +9536,66 @@
       <c r="A1" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="293" t="s">
+      <c r="C1" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="293"/>
+      <c r="D1" s="337"/>
       <c r="E1" s="287"/>
       <c r="F1" s="287"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="294" t="s">
+      <c r="H1" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="294"/>
+      <c r="I1" s="338"/>
       <c r="J1" s="287"/>
       <c r="K1" s="287"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="295" t="s">
+      <c r="M1" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="295"/>
+      <c r="N1" s="339"/>
       <c r="O1" s="287"/>
       <c r="P1" s="287"/>
       <c r="Q1" s="7"/>
-      <c r="R1" s="296" t="s">
+      <c r="R1" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="296"/>
+      <c r="S1" s="340"/>
       <c r="T1" s="287"/>
       <c r="U1" s="287"/>
       <c r="V1" s="7"/>
-      <c r="W1" s="297" t="s">
+      <c r="W1" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="297"/>
+      <c r="X1" s="341"/>
       <c r="Y1" s="287"/>
       <c r="Z1" s="287"/>
       <c r="AA1" s="7"/>
-      <c r="AB1" s="290" t="s">
+      <c r="AB1" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" s="291"/>
+      <c r="AC1" s="335"/>
       <c r="AD1" s="287"/>
       <c r="AE1" s="287"/>
       <c r="AF1" s="7"/>
-      <c r="AG1" s="292" t="s">
+      <c r="AG1" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" s="298"/>
+      <c r="AH1" s="343"/>
       <c r="AI1" s="287"/>
       <c r="AJ1" s="287"/>
       <c r="AK1" s="7"/>
-      <c r="AL1" s="299" t="s">
+      <c r="AL1" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM1" s="299"/>
+      <c r="AM1" s="336"/>
       <c r="AN1" s="287"/>
       <c r="AO1" s="287"/>
       <c r="AP1" s="7"/>
-      <c r="AQ1" s="300" t="s">
+      <c r="AQ1" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR1" s="300"/>
+      <c r="AR1" s="345"/>
       <c r="AS1" s="287"/>
       <c r="AT1" s="287"/>
       <c r="AU1" s="7"/>
@@ -9610,66 +9610,66 @@
       <c r="B2" s="276"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
-      <c r="E2" s="289" t="s">
+      <c r="E2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="289"/>
+      <c r="F2" s="333"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
-      <c r="J2" s="289" t="s">
+      <c r="J2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="289"/>
+      <c r="K2" s="333"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
-      <c r="O2" s="289" t="s">
+      <c r="O2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P2" s="289"/>
+      <c r="P2" s="333"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
-      <c r="T2" s="289" t="s">
+      <c r="T2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U2" s="289"/>
+      <c r="U2" s="333"/>
       <c r="V2" s="22"/>
       <c r="W2" s="22"/>
       <c r="X2" s="22"/>
-      <c r="Y2" s="289" t="s">
+      <c r="Y2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z2" s="289"/>
+      <c r="Z2" s="333"/>
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
       <c r="AC2" s="22"/>
-      <c r="AD2" s="289" t="s">
+      <c r="AD2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE2" s="289"/>
+      <c r="AE2" s="333"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="22"/>
       <c r="AH2" s="22"/>
-      <c r="AI2" s="289" t="s">
+      <c r="AI2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ2" s="289"/>
+      <c r="AJ2" s="333"/>
       <c r="AK2" s="22"/>
       <c r="AL2" s="22"/>
       <c r="AM2" s="22"/>
-      <c r="AN2" s="289" t="s">
+      <c r="AN2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO2" s="289"/>
+      <c r="AO2" s="333"/>
       <c r="AP2" s="22"/>
       <c r="AQ2" s="22"/>
       <c r="AR2" s="22"/>
-      <c r="AS2" s="289" t="s">
+      <c r="AS2" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT2" s="289"/>
+      <c r="AT2" s="333"/>
       <c r="AU2" s="22"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.15">
@@ -10826,50 +10826,50 @@
       <c r="A24" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="293" t="s">
+      <c r="C24" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="293"/>
+      <c r="D24" s="337"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="294" t="s">
+      <c r="H24" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="294"/>
+      <c r="I24" s="338"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="295" t="s">
+      <c r="M24" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N24" s="295"/>
+      <c r="N24" s="339"/>
       <c r="Q24" s="7"/>
-      <c r="R24" s="296" t="s">
+      <c r="R24" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S24" s="296"/>
+      <c r="S24" s="340"/>
       <c r="V24" s="7"/>
-      <c r="W24" s="297" t="s">
+      <c r="W24" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X24" s="297"/>
+      <c r="X24" s="341"/>
       <c r="AA24" s="7"/>
-      <c r="AB24" s="290" t="s">
+      <c r="AB24" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC24" s="291"/>
+      <c r="AC24" s="335"/>
       <c r="AF24" s="7"/>
-      <c r="AG24" s="292" t="s">
+      <c r="AG24" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH24" s="298"/>
+      <c r="AH24" s="343"/>
       <c r="AK24" s="7"/>
-      <c r="AL24" s="299" t="s">
+      <c r="AL24" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM24" s="299"/>
+      <c r="AM24" s="336"/>
       <c r="AP24" s="7"/>
-      <c r="AQ24" s="300" t="s">
+      <c r="AQ24" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR24" s="300"/>
+      <c r="AR24" s="345"/>
       <c r="AU24" s="7"/>
     </row>
     <row r="25" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -10879,66 +10879,66 @@
       <c r="B25" s="278"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
-      <c r="E25" s="289" t="s">
+      <c r="E25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F25" s="289"/>
+      <c r="F25" s="333"/>
       <c r="G25" s="23"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="289" t="s">
+      <c r="J25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="289"/>
+      <c r="K25" s="333"/>
       <c r="L25" s="23"/>
       <c r="M25" s="23"/>
       <c r="N25" s="23"/>
-      <c r="O25" s="289" t="s">
+      <c r="O25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P25" s="289"/>
+      <c r="P25" s="333"/>
       <c r="Q25" s="23"/>
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
-      <c r="T25" s="289" t="s">
+      <c r="T25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U25" s="289"/>
+      <c r="U25" s="333"/>
       <c r="V25" s="23"/>
       <c r="W25" s="23"/>
       <c r="X25" s="23"/>
-      <c r="Y25" s="289" t="s">
+      <c r="Y25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z25" s="289"/>
+      <c r="Z25" s="333"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
       <c r="AC25" s="23"/>
-      <c r="AD25" s="289" t="s">
+      <c r="AD25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE25" s="289"/>
+      <c r="AE25" s="333"/>
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
       <c r="AH25" s="23"/>
-      <c r="AI25" s="289" t="s">
+      <c r="AI25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ25" s="289"/>
+      <c r="AJ25" s="333"/>
       <c r="AK25" s="23"/>
       <c r="AL25" s="23"/>
       <c r="AM25" s="23"/>
-      <c r="AN25" s="289" t="s">
+      <c r="AN25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO25" s="289"/>
+      <c r="AO25" s="333"/>
       <c r="AP25" s="23"/>
       <c r="AQ25" s="23"/>
       <c r="AR25" s="23"/>
-      <c r="AS25" s="289" t="s">
+      <c r="AS25" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT25" s="289"/>
+      <c r="AT25" s="333"/>
       <c r="AU25" s="23"/>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.15">
@@ -12319,50 +12319,50 @@
       <c r="A47" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="293" t="s">
+      <c r="C47" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="293"/>
+      <c r="D47" s="337"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="294" t="s">
+      <c r="H47" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I47" s="294"/>
+      <c r="I47" s="338"/>
       <c r="L47" s="7"/>
-      <c r="M47" s="295" t="s">
+      <c r="M47" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N47" s="295"/>
+      <c r="N47" s="339"/>
       <c r="Q47" s="7"/>
-      <c r="R47" s="296" t="s">
+      <c r="R47" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S47" s="296"/>
+      <c r="S47" s="340"/>
       <c r="V47" s="7"/>
-      <c r="W47" s="297" t="s">
+      <c r="W47" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X47" s="297"/>
+      <c r="X47" s="341"/>
       <c r="AA47" s="7"/>
-      <c r="AB47" s="290" t="s">
+      <c r="AB47" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC47" s="291"/>
+      <c r="AC47" s="335"/>
       <c r="AF47" s="7"/>
-      <c r="AG47" s="292" t="s">
+      <c r="AG47" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH47" s="298"/>
+      <c r="AH47" s="343"/>
       <c r="AK47" s="7"/>
-      <c r="AL47" s="299" t="s">
+      <c r="AL47" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM47" s="299"/>
+      <c r="AM47" s="336"/>
       <c r="AP47" s="7"/>
-      <c r="AQ47" s="300" t="s">
+      <c r="AQ47" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR47" s="300"/>
+      <c r="AR47" s="345"/>
       <c r="AU47" s="7"/>
     </row>
     <row r="48" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -12372,66 +12372,66 @@
       <c r="B48" s="279"/>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
-      <c r="E48" s="289" t="s">
+      <c r="E48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F48" s="289"/>
+      <c r="F48" s="333"/>
       <c r="G48" s="23"/>
       <c r="H48" s="25"/>
       <c r="I48" s="25"/>
-      <c r="J48" s="289" t="s">
+      <c r="J48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K48" s="289"/>
+      <c r="K48" s="333"/>
       <c r="L48" s="23"/>
       <c r="M48" s="25"/>
       <c r="N48" s="25"/>
-      <c r="O48" s="289" t="s">
+      <c r="O48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P48" s="289"/>
+      <c r="P48" s="333"/>
       <c r="Q48" s="23"/>
       <c r="R48" s="23"/>
       <c r="S48" s="23"/>
-      <c r="T48" s="289" t="s">
+      <c r="T48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U48" s="289"/>
+      <c r="U48" s="333"/>
       <c r="V48" s="23"/>
       <c r="W48" s="23"/>
       <c r="X48" s="23"/>
-      <c r="Y48" s="289" t="s">
+      <c r="Y48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z48" s="289"/>
+      <c r="Z48" s="333"/>
       <c r="AA48" s="23"/>
       <c r="AB48" s="23"/>
       <c r="AC48" s="23"/>
-      <c r="AD48" s="289" t="s">
+      <c r="AD48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE48" s="289"/>
+      <c r="AE48" s="333"/>
       <c r="AF48" s="23"/>
       <c r="AG48" s="23"/>
       <c r="AH48" s="23"/>
-      <c r="AI48" s="289" t="s">
+      <c r="AI48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ48" s="289"/>
+      <c r="AJ48" s="333"/>
       <c r="AK48" s="23"/>
       <c r="AL48" s="25"/>
       <c r="AM48" s="25"/>
-      <c r="AN48" s="289" t="s">
+      <c r="AN48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO48" s="289"/>
+      <c r="AO48" s="333"/>
       <c r="AP48" s="23"/>
       <c r="AQ48" s="25"/>
       <c r="AR48" s="25"/>
-      <c r="AS48" s="289" t="s">
+      <c r="AS48" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT48" s="289"/>
+      <c r="AT48" s="333"/>
       <c r="AU48" s="25"/>
     </row>
     <row r="49" spans="1:47" x14ac:dyDescent="0.15">
@@ -13930,50 +13930,50 @@
       <c r="A70" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="293" t="s">
+      <c r="C70" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="293"/>
+      <c r="D70" s="337"/>
       <c r="G70" s="7"/>
-      <c r="H70" s="294" t="s">
+      <c r="H70" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I70" s="294"/>
+      <c r="I70" s="338"/>
       <c r="L70" s="7"/>
-      <c r="M70" s="295" t="s">
+      <c r="M70" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N70" s="295"/>
+      <c r="N70" s="339"/>
       <c r="Q70" s="7"/>
-      <c r="R70" s="296" t="s">
+      <c r="R70" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S70" s="296"/>
+      <c r="S70" s="340"/>
       <c r="V70" s="7"/>
-      <c r="W70" s="297" t="s">
+      <c r="W70" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X70" s="297"/>
+      <c r="X70" s="341"/>
       <c r="AA70" s="7"/>
-      <c r="AB70" s="290" t="s">
+      <c r="AB70" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC70" s="291"/>
+      <c r="AC70" s="335"/>
       <c r="AF70" s="7"/>
-      <c r="AG70" s="292" t="s">
+      <c r="AG70" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH70" s="298"/>
+      <c r="AH70" s="343"/>
       <c r="AK70" s="7"/>
-      <c r="AL70" s="299" t="s">
+      <c r="AL70" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM70" s="299"/>
+      <c r="AM70" s="336"/>
       <c r="AP70" s="7"/>
-      <c r="AQ70" s="300" t="s">
+      <c r="AQ70" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR70" s="300"/>
+      <c r="AR70" s="345"/>
       <c r="AU70" s="7"/>
     </row>
     <row r="71" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -13983,66 +13983,66 @@
       <c r="B71" s="278"/>
       <c r="C71" s="23"/>
       <c r="D71" s="23"/>
-      <c r="E71" s="289" t="s">
+      <c r="E71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F71" s="289"/>
+      <c r="F71" s="333"/>
       <c r="G71" s="23"/>
       <c r="H71" s="25"/>
       <c r="I71" s="25"/>
-      <c r="J71" s="289" t="s">
+      <c r="J71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K71" s="289"/>
+      <c r="K71" s="333"/>
       <c r="L71" s="23"/>
       <c r="M71" s="23"/>
       <c r="N71" s="23"/>
-      <c r="O71" s="289" t="s">
+      <c r="O71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P71" s="289"/>
+      <c r="P71" s="333"/>
       <c r="Q71" s="23"/>
       <c r="R71" s="23"/>
       <c r="S71" s="23"/>
-      <c r="T71" s="289" t="s">
+      <c r="T71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U71" s="289"/>
+      <c r="U71" s="333"/>
       <c r="V71" s="23"/>
       <c r="W71" s="23"/>
       <c r="X71" s="23"/>
-      <c r="Y71" s="289" t="s">
+      <c r="Y71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z71" s="289"/>
+      <c r="Z71" s="333"/>
       <c r="AA71" s="23"/>
       <c r="AB71" s="23"/>
       <c r="AC71" s="23"/>
-      <c r="AD71" s="289" t="s">
+      <c r="AD71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE71" s="289"/>
+      <c r="AE71" s="333"/>
       <c r="AF71" s="23"/>
       <c r="AG71" s="23"/>
       <c r="AH71" s="23"/>
-      <c r="AI71" s="289" t="s">
+      <c r="AI71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ71" s="289"/>
+      <c r="AJ71" s="333"/>
       <c r="AK71" s="23"/>
       <c r="AL71" s="23"/>
       <c r="AM71" s="23"/>
-      <c r="AN71" s="289" t="s">
+      <c r="AN71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO71" s="289"/>
+      <c r="AO71" s="333"/>
       <c r="AP71" s="23"/>
       <c r="AQ71" s="23"/>
       <c r="AR71" s="23"/>
-      <c r="AS71" s="289" t="s">
+      <c r="AS71" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT71" s="289"/>
+      <c r="AT71" s="333"/>
       <c r="AU71" s="23"/>
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.15">
@@ -15545,50 +15545,50 @@
       <c r="A93" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="293" t="s">
+      <c r="C93" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="293"/>
+      <c r="D93" s="337"/>
       <c r="G93" s="7"/>
-      <c r="H93" s="294" t="s">
+      <c r="H93" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I93" s="294"/>
+      <c r="I93" s="338"/>
       <c r="L93" s="7"/>
-      <c r="M93" s="295" t="s">
+      <c r="M93" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N93" s="295"/>
+      <c r="N93" s="339"/>
       <c r="Q93" s="7"/>
-      <c r="R93" s="296" t="s">
+      <c r="R93" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S93" s="296"/>
+      <c r="S93" s="340"/>
       <c r="V93" s="7"/>
-      <c r="W93" s="297" t="s">
+      <c r="W93" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X93" s="297"/>
+      <c r="X93" s="341"/>
       <c r="AA93" s="7"/>
-      <c r="AB93" s="290" t="s">
+      <c r="AB93" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC93" s="291"/>
+      <c r="AC93" s="335"/>
       <c r="AF93" s="7"/>
-      <c r="AG93" s="292" t="s">
+      <c r="AG93" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH93" s="298"/>
+      <c r="AH93" s="343"/>
       <c r="AK93" s="7"/>
-      <c r="AL93" s="299" t="s">
+      <c r="AL93" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM93" s="299"/>
+      <c r="AM93" s="336"/>
       <c r="AP93" s="7"/>
-      <c r="AQ93" s="300" t="s">
+      <c r="AQ93" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR93" s="300"/>
+      <c r="AR93" s="345"/>
       <c r="AU93" s="7"/>
     </row>
     <row r="94" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -15598,66 +15598,66 @@
       <c r="B94" s="278"/>
       <c r="C94" s="25"/>
       <c r="D94" s="25"/>
-      <c r="E94" s="289" t="s">
+      <c r="E94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F94" s="289"/>
+      <c r="F94" s="333"/>
       <c r="G94" s="24"/>
       <c r="H94" s="24"/>
       <c r="I94" s="24"/>
-      <c r="J94" s="289" t="s">
+      <c r="J94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K94" s="289"/>
+      <c r="K94" s="333"/>
       <c r="L94" s="24"/>
       <c r="M94" s="24"/>
       <c r="N94" s="24"/>
-      <c r="O94" s="289" t="s">
+      <c r="O94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P94" s="289"/>
+      <c r="P94" s="333"/>
       <c r="Q94" s="24"/>
       <c r="R94" s="24"/>
       <c r="S94" s="24"/>
-      <c r="T94" s="289" t="s">
+      <c r="T94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U94" s="289"/>
+      <c r="U94" s="333"/>
       <c r="V94" s="24"/>
       <c r="W94" s="24"/>
       <c r="X94" s="24"/>
-      <c r="Y94" s="289" t="s">
+      <c r="Y94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z94" s="289"/>
+      <c r="Z94" s="333"/>
       <c r="AA94" s="24"/>
       <c r="AB94" s="24"/>
       <c r="AC94" s="24"/>
-      <c r="AD94" s="289" t="s">
+      <c r="AD94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE94" s="289"/>
+      <c r="AE94" s="333"/>
       <c r="AF94" s="24"/>
       <c r="AG94" s="24"/>
       <c r="AH94" s="24"/>
-      <c r="AI94" s="289" t="s">
+      <c r="AI94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ94" s="289"/>
+      <c r="AJ94" s="333"/>
       <c r="AK94" s="24"/>
       <c r="AL94" s="24"/>
       <c r="AM94" s="24"/>
-      <c r="AN94" s="289" t="s">
+      <c r="AN94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO94" s="289"/>
+      <c r="AO94" s="333"/>
       <c r="AP94" s="24"/>
       <c r="AQ94" s="24"/>
       <c r="AR94" s="24"/>
-      <c r="AS94" s="289" t="s">
+      <c r="AS94" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT94" s="289"/>
+      <c r="AT94" s="333"/>
       <c r="AU94" s="24"/>
     </row>
     <row r="95" spans="1:49" x14ac:dyDescent="0.15">
@@ -17206,50 +17206,50 @@
       <c r="A116" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C116" s="293" t="s">
+      <c r="C116" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D116" s="293"/>
+      <c r="D116" s="337"/>
       <c r="G116" s="7"/>
-      <c r="H116" s="294" t="s">
+      <c r="H116" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I116" s="294"/>
+      <c r="I116" s="338"/>
       <c r="L116" s="7"/>
-      <c r="M116" s="295" t="s">
+      <c r="M116" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N116" s="295"/>
+      <c r="N116" s="339"/>
       <c r="Q116" s="7"/>
-      <c r="R116" s="296" t="s">
+      <c r="R116" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S116" s="296"/>
+      <c r="S116" s="340"/>
       <c r="V116" s="7"/>
-      <c r="W116" s="297" t="s">
+      <c r="W116" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X116" s="297"/>
+      <c r="X116" s="341"/>
       <c r="AA116" s="7"/>
-      <c r="AB116" s="290" t="s">
+      <c r="AB116" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC116" s="291"/>
+      <c r="AC116" s="335"/>
       <c r="AF116" s="7"/>
-      <c r="AG116" s="292" t="s">
+      <c r="AG116" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH116" s="298"/>
+      <c r="AH116" s="343"/>
       <c r="AK116" s="7"/>
-      <c r="AL116" s="299" t="s">
+      <c r="AL116" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM116" s="299"/>
+      <c r="AM116" s="336"/>
       <c r="AP116" s="7"/>
-      <c r="AQ116" s="300" t="s">
+      <c r="AQ116" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR116" s="300"/>
+      <c r="AR116" s="345"/>
       <c r="AU116" s="7"/>
     </row>
     <row r="117" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -17259,66 +17259,66 @@
       <c r="B117" s="278"/>
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
-      <c r="E117" s="289" t="s">
+      <c r="E117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F117" s="289"/>
+      <c r="F117" s="333"/>
       <c r="G117" s="24"/>
       <c r="H117" s="24"/>
       <c r="I117" s="24"/>
-      <c r="J117" s="289" t="s">
+      <c r="J117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K117" s="289"/>
+      <c r="K117" s="333"/>
       <c r="L117" s="24"/>
       <c r="M117" s="24"/>
       <c r="N117" s="24"/>
-      <c r="O117" s="289" t="s">
+      <c r="O117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P117" s="289"/>
+      <c r="P117" s="333"/>
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
       <c r="S117" s="24"/>
-      <c r="T117" s="289" t="s">
+      <c r="T117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U117" s="289"/>
+      <c r="U117" s="333"/>
       <c r="V117" s="24"/>
       <c r="W117" s="24"/>
       <c r="X117" s="24"/>
-      <c r="Y117" s="289" t="s">
+      <c r="Y117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z117" s="289"/>
+      <c r="Z117" s="333"/>
       <c r="AA117" s="24"/>
       <c r="AB117" s="24"/>
       <c r="AC117" s="24"/>
-      <c r="AD117" s="289" t="s">
+      <c r="AD117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE117" s="289"/>
+      <c r="AE117" s="333"/>
       <c r="AF117" s="24"/>
       <c r="AG117" s="24"/>
       <c r="AH117" s="24"/>
-      <c r="AI117" s="289" t="s">
+      <c r="AI117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ117" s="289"/>
+      <c r="AJ117" s="333"/>
       <c r="AK117" s="24"/>
       <c r="AL117" s="24"/>
       <c r="AM117" s="24"/>
-      <c r="AN117" s="289" t="s">
+      <c r="AN117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO117" s="289"/>
+      <c r="AO117" s="333"/>
       <c r="AP117" s="24"/>
       <c r="AQ117" s="24"/>
       <c r="AR117" s="24"/>
-      <c r="AS117" s="289" t="s">
+      <c r="AS117" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT117" s="289"/>
+      <c r="AT117" s="333"/>
       <c r="AU117" s="24"/>
     </row>
     <row r="118" spans="1:49" x14ac:dyDescent="0.15">
@@ -18883,50 +18883,50 @@
       <c r="A139" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C139" s="293" t="s">
+      <c r="C139" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D139" s="293"/>
+      <c r="D139" s="337"/>
       <c r="G139" s="7"/>
-      <c r="H139" s="294" t="s">
+      <c r="H139" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I139" s="294"/>
+      <c r="I139" s="338"/>
       <c r="L139" s="7"/>
-      <c r="M139" s="295" t="s">
+      <c r="M139" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N139" s="295"/>
+      <c r="N139" s="339"/>
       <c r="Q139" s="7"/>
-      <c r="R139" s="296" t="s">
+      <c r="R139" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S139" s="296"/>
+      <c r="S139" s="340"/>
       <c r="V139" s="7"/>
-      <c r="W139" s="297" t="s">
+      <c r="W139" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X139" s="297"/>
+      <c r="X139" s="341"/>
       <c r="AA139" s="7"/>
-      <c r="AB139" s="290" t="s">
+      <c r="AB139" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC139" s="291"/>
+      <c r="AC139" s="335"/>
       <c r="AF139" s="7"/>
-      <c r="AG139" s="292" t="s">
+      <c r="AG139" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH139" s="298"/>
+      <c r="AH139" s="343"/>
       <c r="AK139" s="7"/>
-      <c r="AL139" s="299" t="s">
+      <c r="AL139" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM139" s="299"/>
+      <c r="AM139" s="336"/>
       <c r="AP139" s="7"/>
-      <c r="AQ139" s="300" t="s">
+      <c r="AQ139" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR139" s="300"/>
+      <c r="AR139" s="345"/>
       <c r="AU139" s="7"/>
     </row>
     <row r="140" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -18936,66 +18936,66 @@
       <c r="B140" s="278"/>
       <c r="C140" s="26"/>
       <c r="D140" s="26"/>
-      <c r="E140" s="289" t="s">
+      <c r="E140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F140" s="289"/>
+      <c r="F140" s="333"/>
       <c r="G140" s="26"/>
       <c r="H140" s="24"/>
       <c r="I140" s="24"/>
-      <c r="J140" s="289" t="s">
+      <c r="J140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K140" s="289"/>
+      <c r="K140" s="333"/>
       <c r="L140" s="26"/>
       <c r="M140" s="24"/>
       <c r="N140" s="24"/>
-      <c r="O140" s="289" t="s">
+      <c r="O140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P140" s="289"/>
+      <c r="P140" s="333"/>
       <c r="Q140" s="26"/>
       <c r="R140" s="26"/>
       <c r="S140" s="26"/>
-      <c r="T140" s="289" t="s">
+      <c r="T140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U140" s="289"/>
+      <c r="U140" s="333"/>
       <c r="V140" s="26"/>
       <c r="W140" s="26"/>
       <c r="X140" s="26"/>
-      <c r="Y140" s="289" t="s">
+      <c r="Y140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z140" s="289"/>
+      <c r="Z140" s="333"/>
       <c r="AA140" s="26"/>
       <c r="AB140" s="26"/>
       <c r="AC140" s="26"/>
-      <c r="AD140" s="289" t="s">
+      <c r="AD140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE140" s="289"/>
+      <c r="AE140" s="333"/>
       <c r="AF140" s="26"/>
       <c r="AG140" s="26"/>
       <c r="AH140" s="26"/>
-      <c r="AI140" s="289" t="s">
+      <c r="AI140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ140" s="289"/>
+      <c r="AJ140" s="333"/>
       <c r="AK140" s="26"/>
       <c r="AL140" s="24"/>
       <c r="AM140" s="24"/>
-      <c r="AN140" s="289" t="s">
+      <c r="AN140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO140" s="289"/>
+      <c r="AO140" s="333"/>
       <c r="AP140" s="26"/>
       <c r="AQ140" s="24"/>
       <c r="AR140" s="24"/>
-      <c r="AS140" s="289" t="s">
+      <c r="AS140" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT140" s="289"/>
+      <c r="AT140" s="333"/>
       <c r="AU140" s="24"/>
     </row>
     <row r="141" spans="1:49" x14ac:dyDescent="0.15">
@@ -20478,50 +20478,50 @@
       <c r="A162" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C162" s="293" t="s">
+      <c r="C162" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D162" s="293"/>
+      <c r="D162" s="337"/>
       <c r="G162" s="7"/>
-      <c r="H162" s="294" t="s">
+      <c r="H162" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I162" s="294"/>
+      <c r="I162" s="338"/>
       <c r="L162" s="7"/>
-      <c r="M162" s="295" t="s">
+      <c r="M162" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N162" s="295"/>
+      <c r="N162" s="339"/>
       <c r="Q162" s="7"/>
-      <c r="R162" s="296" t="s">
+      <c r="R162" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S162" s="296"/>
+      <c r="S162" s="340"/>
       <c r="V162" s="7"/>
-      <c r="W162" s="297" t="s">
+      <c r="W162" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X162" s="297"/>
+      <c r="X162" s="341"/>
       <c r="AA162" s="7"/>
-      <c r="AB162" s="290" t="s">
+      <c r="AB162" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC162" s="291"/>
+      <c r="AC162" s="335"/>
       <c r="AF162" s="7"/>
-      <c r="AG162" s="292" t="s">
+      <c r="AG162" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH162" s="298"/>
+      <c r="AH162" s="343"/>
       <c r="AK162" s="7"/>
-      <c r="AL162" s="299" t="s">
+      <c r="AL162" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM162" s="299"/>
+      <c r="AM162" s="336"/>
       <c r="AP162" s="7"/>
-      <c r="AQ162" s="300" t="s">
+      <c r="AQ162" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR162" s="300"/>
+      <c r="AR162" s="345"/>
       <c r="AU162" s="7"/>
     </row>
     <row r="163" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -20531,66 +20531,66 @@
       <c r="B163" s="278"/>
       <c r="C163" s="26"/>
       <c r="D163" s="26"/>
-      <c r="E163" s="289" t="s">
+      <c r="E163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F163" s="289"/>
+      <c r="F163" s="333"/>
       <c r="G163" s="26"/>
       <c r="H163" s="24"/>
       <c r="I163" s="24"/>
-      <c r="J163" s="289" t="s">
+      <c r="J163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K163" s="289"/>
+      <c r="K163" s="333"/>
       <c r="L163" s="26"/>
       <c r="M163" s="24"/>
       <c r="N163" s="24"/>
-      <c r="O163" s="289" t="s">
+      <c r="O163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P163" s="289"/>
+      <c r="P163" s="333"/>
       <c r="Q163" s="26"/>
       <c r="R163" s="26"/>
       <c r="S163" s="26"/>
-      <c r="T163" s="289" t="s">
+      <c r="T163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U163" s="289"/>
+      <c r="U163" s="333"/>
       <c r="V163" s="26"/>
       <c r="W163" s="26"/>
       <c r="X163" s="26"/>
-      <c r="Y163" s="289" t="s">
+      <c r="Y163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z163" s="289"/>
+      <c r="Z163" s="333"/>
       <c r="AA163" s="26"/>
       <c r="AB163" s="26"/>
       <c r="AC163" s="26"/>
-      <c r="AD163" s="289" t="s">
+      <c r="AD163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE163" s="289"/>
+      <c r="AE163" s="333"/>
       <c r="AF163" s="26"/>
       <c r="AG163" s="26"/>
       <c r="AH163" s="26"/>
-      <c r="AI163" s="289" t="s">
+      <c r="AI163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ163" s="289"/>
+      <c r="AJ163" s="333"/>
       <c r="AK163" s="26"/>
       <c r="AL163" s="24"/>
       <c r="AM163" s="24"/>
-      <c r="AN163" s="289" t="s">
+      <c r="AN163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO163" s="289"/>
+      <c r="AO163" s="333"/>
       <c r="AP163" s="26"/>
       <c r="AQ163" s="24"/>
       <c r="AR163" s="24"/>
-      <c r="AS163" s="289" t="s">
+      <c r="AS163" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT163" s="289"/>
+      <c r="AT163" s="333"/>
       <c r="AU163" s="24"/>
     </row>
     <row r="164" spans="1:49" x14ac:dyDescent="0.15">
@@ -21843,50 +21843,50 @@
       <c r="A185" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C185" s="293" t="s">
+      <c r="C185" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D185" s="293"/>
+      <c r="D185" s="337"/>
       <c r="G185" s="7"/>
-      <c r="H185" s="294" t="s">
+      <c r="H185" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I185" s="294"/>
+      <c r="I185" s="338"/>
       <c r="L185" s="7"/>
-      <c r="M185" s="295" t="s">
+      <c r="M185" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N185" s="295"/>
+      <c r="N185" s="339"/>
       <c r="Q185" s="7"/>
-      <c r="R185" s="296" t="s">
+      <c r="R185" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S185" s="296"/>
+      <c r="S185" s="340"/>
       <c r="V185" s="7"/>
-      <c r="W185" s="297" t="s">
+      <c r="W185" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X185" s="297"/>
+      <c r="X185" s="341"/>
       <c r="AA185" s="7"/>
-      <c r="AB185" s="290" t="s">
+      <c r="AB185" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC185" s="291"/>
+      <c r="AC185" s="335"/>
       <c r="AF185" s="7"/>
-      <c r="AG185" s="292" t="s">
+      <c r="AG185" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH185" s="298"/>
+      <c r="AH185" s="343"/>
       <c r="AK185" s="7"/>
-      <c r="AL185" s="299" t="s">
+      <c r="AL185" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM185" s="299"/>
+      <c r="AM185" s="336"/>
       <c r="AP185" s="7"/>
-      <c r="AQ185" s="300" t="s">
+      <c r="AQ185" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR185" s="300"/>
+      <c r="AR185" s="345"/>
       <c r="AU185" s="7"/>
     </row>
     <row r="186" spans="1:49" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -21896,66 +21896,66 @@
       <c r="B186" s="278"/>
       <c r="C186" s="24"/>
       <c r="D186" s="24"/>
-      <c r="E186" s="289" t="s">
+      <c r="E186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F186" s="289"/>
+      <c r="F186" s="333"/>
       <c r="G186" s="24"/>
       <c r="H186" s="24"/>
       <c r="I186" s="24"/>
-      <c r="J186" s="289" t="s">
+      <c r="J186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K186" s="289"/>
+      <c r="K186" s="333"/>
       <c r="L186" s="24"/>
       <c r="M186" s="26"/>
       <c r="N186" s="26"/>
-      <c r="O186" s="289" t="s">
+      <c r="O186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P186" s="289"/>
+      <c r="P186" s="333"/>
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
       <c r="S186" s="24"/>
-      <c r="T186" s="289" t="s">
+      <c r="T186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U186" s="289"/>
+      <c r="U186" s="333"/>
       <c r="V186" s="24"/>
       <c r="W186" s="24"/>
       <c r="X186" s="24"/>
-      <c r="Y186" s="289" t="s">
+      <c r="Y186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z186" s="289"/>
+      <c r="Z186" s="333"/>
       <c r="AA186" s="24"/>
       <c r="AB186" s="24"/>
       <c r="AC186" s="24"/>
-      <c r="AD186" s="289" t="s">
+      <c r="AD186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE186" s="289"/>
+      <c r="AE186" s="333"/>
       <c r="AF186" s="24"/>
       <c r="AG186" s="24"/>
       <c r="AH186" s="24"/>
-      <c r="AI186" s="289" t="s">
+      <c r="AI186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ186" s="289"/>
+      <c r="AJ186" s="333"/>
       <c r="AK186" s="24"/>
       <c r="AL186" s="26"/>
       <c r="AM186" s="26"/>
-      <c r="AN186" s="289" t="s">
+      <c r="AN186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO186" s="289"/>
+      <c r="AO186" s="333"/>
       <c r="AP186" s="24"/>
       <c r="AQ186" s="26"/>
       <c r="AR186" s="26"/>
-      <c r="AS186" s="289" t="s">
+      <c r="AS186" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT186" s="289"/>
+      <c r="AT186" s="333"/>
       <c r="AU186" s="26"/>
     </row>
     <row r="187" spans="1:49" x14ac:dyDescent="0.15">
@@ -23110,50 +23110,50 @@
       <c r="A208" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C208" s="293" t="s">
+      <c r="C208" s="337" t="s">
         <v>5</v>
       </c>
-      <c r="D208" s="293"/>
+      <c r="D208" s="337"/>
       <c r="G208" s="7"/>
-      <c r="H208" s="294" t="s">
+      <c r="H208" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I208" s="294"/>
+      <c r="I208" s="338"/>
       <c r="L208" s="7"/>
-      <c r="M208" s="295" t="s">
+      <c r="M208" s="339" t="s">
         <v>4</v>
       </c>
-      <c r="N208" s="295"/>
+      <c r="N208" s="339"/>
       <c r="Q208" s="7"/>
-      <c r="R208" s="296" t="s">
+      <c r="R208" s="340" t="s">
         <v>7</v>
       </c>
-      <c r="S208" s="296"/>
+      <c r="S208" s="340"/>
       <c r="V208" s="7"/>
-      <c r="W208" s="297" t="s">
+      <c r="W208" s="341" t="s">
         <v>8</v>
       </c>
-      <c r="X208" s="297"/>
+      <c r="X208" s="341"/>
       <c r="AA208" s="7"/>
-      <c r="AB208" s="290" t="s">
+      <c r="AB208" s="334" t="s">
         <v>9</v>
       </c>
-      <c r="AC208" s="290"/>
+      <c r="AC208" s="334"/>
       <c r="AF208" s="7"/>
-      <c r="AG208" s="292" t="s">
+      <c r="AG208" s="342" t="s">
         <v>10</v>
       </c>
-      <c r="AH208" s="292"/>
+      <c r="AH208" s="342"/>
       <c r="AK208" s="7"/>
-      <c r="AL208" s="299" t="s">
+      <c r="AL208" s="336" t="s">
         <v>12</v>
       </c>
-      <c r="AM208" s="299"/>
+      <c r="AM208" s="336"/>
       <c r="AP208" s="7"/>
-      <c r="AQ208" s="300" t="s">
+      <c r="AQ208" s="345" t="s">
         <v>13</v>
       </c>
-      <c r="AR208" s="300"/>
+      <c r="AR208" s="345"/>
       <c r="AU208" s="7"/>
     </row>
     <row r="209" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -23163,66 +23163,66 @@
       <c r="B209" s="276"/>
       <c r="C209" s="24"/>
       <c r="D209" s="24"/>
-      <c r="E209" s="289" t="s">
+      <c r="E209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F209" s="289"/>
+      <c r="F209" s="333"/>
       <c r="G209" s="24"/>
       <c r="H209" s="26"/>
       <c r="I209" s="26"/>
-      <c r="J209" s="289" t="s">
+      <c r="J209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K209" s="289"/>
+      <c r="K209" s="333"/>
       <c r="L209" s="26"/>
       <c r="M209" s="24"/>
       <c r="N209" s="24"/>
-      <c r="O209" s="289" t="s">
+      <c r="O209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="P209" s="289"/>
+      <c r="P209" s="333"/>
       <c r="Q209" s="26"/>
       <c r="R209" s="26"/>
       <c r="S209" s="26"/>
-      <c r="T209" s="289" t="s">
+      <c r="T209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="U209" s="289"/>
+      <c r="U209" s="333"/>
       <c r="V209" s="26"/>
       <c r="W209" s="26"/>
       <c r="X209" s="26"/>
-      <c r="Y209" s="289" t="s">
+      <c r="Y209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="Z209" s="289"/>
+      <c r="Z209" s="333"/>
       <c r="AA209" s="26"/>
       <c r="AB209" s="26"/>
       <c r="AC209" s="26"/>
-      <c r="AD209" s="289" t="s">
+      <c r="AD209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AE209" s="289"/>
+      <c r="AE209" s="333"/>
       <c r="AF209" s="26"/>
       <c r="AG209" s="26"/>
       <c r="AH209" s="26"/>
-      <c r="AI209" s="289" t="s">
+      <c r="AI209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AJ209" s="289"/>
+      <c r="AJ209" s="333"/>
       <c r="AK209" s="26"/>
       <c r="AL209" s="24"/>
       <c r="AM209" s="24"/>
-      <c r="AN209" s="289" t="s">
+      <c r="AN209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AO209" s="289"/>
+      <c r="AO209" s="333"/>
       <c r="AP209" s="26"/>
       <c r="AQ209" s="24"/>
       <c r="AR209" s="24"/>
-      <c r="AS209" s="289" t="s">
+      <c r="AS209" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="AT209" s="289"/>
+      <c r="AT209" s="333"/>
       <c r="AU209" s="24"/>
     </row>
     <row r="210" spans="1:47" x14ac:dyDescent="0.15">
@@ -24373,21 +24373,21 @@
       <c r="A231" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C231" s="300" t="s">
+      <c r="C231" s="345" t="s">
         <v>245</v>
       </c>
-      <c r="D231" s="300"/>
+      <c r="D231" s="345"/>
       <c r="G231" s="7"/>
-      <c r="H231" s="300" t="s">
+      <c r="H231" s="345" t="s">
         <v>246</v>
       </c>
-      <c r="I231" s="300"/>
+      <c r="I231" s="345"/>
       <c r="L231" s="7"/>
-      <c r="M231" s="345"/>
-      <c r="N231" s="345"/>
+      <c r="M231" s="344"/>
+      <c r="N231" s="344"/>
       <c r="Q231" s="7"/>
-      <c r="R231" s="345"/>
-      <c r="S231" s="345"/>
+      <c r="R231" s="344"/>
+      <c r="S231" s="344"/>
       <c r="V231" s="7"/>
     </row>
     <row r="232" spans="1:49" x14ac:dyDescent="0.15">
@@ -24397,27 +24397,27 @@
       <c r="B232" s="276"/>
       <c r="C232" s="24"/>
       <c r="D232" s="24"/>
-      <c r="E232" s="289" t="s">
+      <c r="E232" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F232" s="289"/>
+      <c r="F232" s="333"/>
       <c r="G232" s="24"/>
       <c r="H232" s="24"/>
       <c r="I232" s="24"/>
-      <c r="J232" s="289" t="s">
+      <c r="J232" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K232" s="289"/>
+      <c r="K232" s="333"/>
       <c r="L232" s="24"/>
       <c r="M232" s="6"/>
       <c r="N232" s="6"/>
-      <c r="O232" s="289"/>
-      <c r="P232" s="289"/>
+      <c r="O232" s="333"/>
+      <c r="P232" s="333"/>
       <c r="Q232" s="6"/>
       <c r="R232" s="6"/>
       <c r="S232" s="6"/>
-      <c r="T232" s="289"/>
-      <c r="U232" s="289"/>
+      <c r="T232" s="333"/>
+      <c r="U232" s="333"/>
       <c r="V232" s="6"/>
     </row>
     <row r="233" spans="1:49" x14ac:dyDescent="0.15">
@@ -24657,20 +24657,28 @@
       <c r="T239" s="284"/>
       <c r="U239" s="284"/>
       <c r="V239" s="6"/>
+      <c r="AV239">
+        <f>SUM(C239,H239,M239,R239,W239,AB239,AG239,AL239,AQ239)</f>
+        <v>10</v>
+      </c>
+      <c r="AW239">
+        <f>SUM(D239,I239,N239,S239,X239,AC239,AH239,AM239,AR239)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="240" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A240" s="275" t="s">
         <v>11</v>
       </c>
-      <c r="C240" s="293" t="s">
+      <c r="C240" s="337" t="s">
         <v>243</v>
       </c>
-      <c r="D240" s="293"/>
+      <c r="D240" s="337"/>
       <c r="G240" s="7"/>
-      <c r="H240" s="293" t="s">
+      <c r="H240" s="337" t="s">
         <v>244</v>
       </c>
-      <c r="I240" s="293"/>
+      <c r="I240" s="337"/>
       <c r="L240" s="7"/>
       <c r="M240" s="6"/>
       <c r="N240" s="6"/>
@@ -24690,17 +24698,17 @@
       <c r="B241" s="276"/>
       <c r="C241" s="24"/>
       <c r="D241" s="24"/>
-      <c r="E241" s="289" t="s">
+      <c r="E241" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="F241" s="289"/>
+      <c r="F241" s="333"/>
       <c r="G241" s="24"/>
       <c r="H241" s="24"/>
       <c r="I241" s="24"/>
-      <c r="J241" s="289" t="s">
+      <c r="J241" s="333" t="s">
         <v>183</v>
       </c>
-      <c r="K241" s="289"/>
+      <c r="K241" s="333"/>
       <c r="L241" s="24"/>
       <c r="M241" s="6"/>
       <c r="N241" s="6"/>
@@ -25076,7 +25084,7 @@
       </c>
       <c r="AV252">
         <f>SUM(AV3:AV248)</f>
-        <v>531</v>
+        <v>541</v>
       </c>
     </row>
     <row r="253" spans="1:49" x14ac:dyDescent="0.15">
@@ -25187,6 +25195,9 @@
     <mergeCell ref="AQ139:AR139"/>
     <mergeCell ref="AQ162:AR162"/>
     <mergeCell ref="AQ185:AR185"/>
+    <mergeCell ref="AG208:AH208"/>
+    <mergeCell ref="O140:P140"/>
+    <mergeCell ref="O209:P209"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="M1:N1"/>
@@ -25241,7 +25252,6 @@
     <mergeCell ref="W116:X116"/>
     <mergeCell ref="E117:F117"/>
     <mergeCell ref="O117:P117"/>
-    <mergeCell ref="AG208:AH208"/>
     <mergeCell ref="C208:D208"/>
     <mergeCell ref="H208:I208"/>
     <mergeCell ref="M208:N208"/>
@@ -25263,6 +25273,8 @@
     <mergeCell ref="W162:X162"/>
     <mergeCell ref="Y163:Z163"/>
     <mergeCell ref="Y186:Z186"/>
+    <mergeCell ref="O163:P163"/>
+    <mergeCell ref="O186:P186"/>
     <mergeCell ref="E140:F140"/>
     <mergeCell ref="E163:F163"/>
     <mergeCell ref="E186:F186"/>
@@ -25282,10 +25294,15 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E71:F71"/>
     <mergeCell ref="E94:F94"/>
-    <mergeCell ref="O140:P140"/>
-    <mergeCell ref="O163:P163"/>
-    <mergeCell ref="O186:P186"/>
-    <mergeCell ref="O209:P209"/>
+    <mergeCell ref="T209:U209"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="O94:P94"/>
+    <mergeCell ref="Y209:Z209"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y25:Z25"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="T25:U25"/>
     <mergeCell ref="T48:U48"/>
@@ -25295,15 +25312,6 @@
     <mergeCell ref="T140:U140"/>
     <mergeCell ref="T163:U163"/>
     <mergeCell ref="T186:U186"/>
-    <mergeCell ref="T209:U209"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="O94:P94"/>
-    <mergeCell ref="Y209:Z209"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y25:Z25"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AD25:AE25"/>
     <mergeCell ref="AD48:AE48"/>
@@ -25322,6 +25330,8 @@
     <mergeCell ref="AB208:AC208"/>
     <mergeCell ref="AB116:AC116"/>
     <mergeCell ref="AN209:AO209"/>
+    <mergeCell ref="AI209:AJ209"/>
+    <mergeCell ref="AL208:AM208"/>
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AN25:AO25"/>
     <mergeCell ref="AN48:AO48"/>
@@ -25331,13 +25341,11 @@
     <mergeCell ref="AI140:AJ140"/>
     <mergeCell ref="AI163:AJ163"/>
     <mergeCell ref="AI186:AJ186"/>
-    <mergeCell ref="AI209:AJ209"/>
     <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="AI25:AJ25"/>
     <mergeCell ref="AI48:AJ48"/>
     <mergeCell ref="AI71:AJ71"/>
     <mergeCell ref="AI94:AJ94"/>
-    <mergeCell ref="AL208:AM208"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.55118110236220474" right="0.55118110236220474" top="0.47244094488188981" bottom="0.43307086614173229" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -25360,215 +25368,215 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="318" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="318" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="306" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="306" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" customWidth="1"/>
     <col min="4" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="319"/>
-      <c r="B1" s="319"/>
+      <c r="A1" s="307"/>
+      <c r="B1" s="307"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="318" t="s">
+      <c r="A2" s="306" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="294" t="s">
+      <c r="D2" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="294"/>
+      <c r="E2" s="338"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="316">
+      <c r="A3" s="304">
         <v>43834</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
+      <c r="B3" s="308"/>
+      <c r="C3" s="309"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="317" t="s">
+      <c r="A4" s="305" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="317" t="s">
+      <c r="B4" s="305" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="322" t="s">
+      <c r="D4" s="310" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="322" t="s">
+      <c r="E4" s="310" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="317" t="s">
+      <c r="A5" s="305" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="317" t="s">
+      <c r="B5" s="305" t="s">
         <v>207</v>
       </c>
-      <c r="D5" s="322" t="s">
+      <c r="D5" s="310" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="322" t="s">
+      <c r="E5" s="310" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="317" t="s">
+      <c r="A6" s="305" t="s">
         <v>208</v>
       </c>
-      <c r="B6" s="317" t="s">
+      <c r="B6" s="305" t="s">
         <v>209</v>
       </c>
-      <c r="D6" s="322" t="s">
+      <c r="D6" s="310" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="322" t="s">
+      <c r="E6" s="310" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="317" t="s">
+      <c r="A7" s="305" t="s">
         <v>201</v>
       </c>
-      <c r="B7" s="317" t="s">
+      <c r="B7" s="305" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="322" t="s">
+      <c r="D7" s="310" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="322" t="s">
+      <c r="E7" s="310" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="317" t="s">
+      <c r="A8" s="305" t="s">
         <v>211</v>
       </c>
-      <c r="B8" s="317" t="s">
+      <c r="B8" s="305" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="322" t="s">
+      <c r="D8" s="310" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="322" t="s">
+      <c r="E8" s="310" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="317" t="s">
+      <c r="A9" s="305" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="317" t="s">
+      <c r="B9" s="305" t="s">
         <v>214</v>
       </c>
-      <c r="D9" s="323" t="s">
+      <c r="D9" s="311" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="323" t="s">
+      <c r="E9" s="311" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="317" t="s">
+      <c r="A10" s="305" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="317" t="s">
+      <c r="B10" s="305" t="s">
         <v>216</v>
       </c>
-      <c r="D10" s="323" t="s">
+      <c r="D10" s="311" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="323" t="s">
+      <c r="E10" s="311" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="317" t="s">
+      <c r="A11" s="305" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="317" t="s">
+      <c r="B11" s="305" t="s">
         <v>218</v>
       </c>
-      <c r="D11" s="323" t="s">
+      <c r="D11" s="311" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="323" t="s">
+      <c r="E11" s="311" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="317" t="s">
+      <c r="A12" s="305" t="s">
         <v>219</v>
       </c>
-      <c r="B12" s="317" t="s">
+      <c r="B12" s="305" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="323" t="s">
+      <c r="D12" s="311" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="323" t="s">
+      <c r="E12" s="311" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="317" t="s">
+      <c r="A13" s="305" t="s">
         <v>221</v>
       </c>
-      <c r="B13" s="317" t="s">
+      <c r="B13" s="305" t="s">
         <v>222</v>
       </c>
-      <c r="D13" s="323" t="s">
+      <c r="D13" s="311" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="323" t="s">
+      <c r="E13" s="311" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="319">
+      <c r="A14" s="307">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B14" s="319">
+      <c r="B14" s="307">
         <v>0.55555555555555558</v>
       </c>
-      <c r="D14" s="324" t="s">
+      <c r="D14" s="312" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="324" t="s">
+      <c r="E14" s="312" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="319">
+      <c r="A15" s="307">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B15" s="319">
+      <c r="B15" s="307">
         <v>0.57222222222222219</v>
       </c>
-      <c r="D15" s="324" t="s">
+      <c r="D15" s="312" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="324" t="s">
+      <c r="E15" s="312" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="319">
+      <c r="A16" s="307">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B16" s="319">
+      <c r="B16" s="307">
         <v>0.58888888888888891</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -25579,580 +25587,580 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="319">
+      <c r="A17" s="307">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B17" s="319">
+      <c r="B17" s="307">
         <v>0.60555555555555551</v>
       </c>
-      <c r="D17" s="324" t="s">
+      <c r="D17" s="312" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="324" t="s">
+      <c r="E17" s="312" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="319">
+      <c r="A18" s="307">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B18" s="319">
+      <c r="B18" s="307">
         <v>0.62222222222222223</v>
       </c>
-      <c r="D18" s="324" t="s">
+      <c r="D18" s="312" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="324" t="s">
+      <c r="E18" s="312" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="319">
+      <c r="A19" s="307">
         <v>0.625</v>
       </c>
-      <c r="B19" s="319">
+      <c r="B19" s="307">
         <v>0.63888888888888895</v>
       </c>
-      <c r="D19" s="324" t="s">
+      <c r="D19" s="312" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="324" t="s">
+      <c r="E19" s="312" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="319">
+      <c r="A20" s="307">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B20" s="319">
+      <c r="B20" s="307">
         <v>0.65555555555555556</v>
       </c>
-      <c r="D20" s="325" t="s">
+      <c r="D20" s="313" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="325" t="s">
+      <c r="E20" s="313" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="319">
+      <c r="A21" s="307">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B21" s="319">
+      <c r="B21" s="307">
         <v>0.67222222222222217</v>
       </c>
-      <c r="D21" s="325" t="s">
+      <c r="D21" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="325" t="s">
+      <c r="E21" s="313" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="319">
+      <c r="A22" s="307">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B22" s="319">
+      <c r="B22" s="307">
         <v>0.68888888888888899</v>
       </c>
-      <c r="D22" s="325" t="s">
+      <c r="D22" s="313" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="325" t="s">
+      <c r="E22" s="313" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="319">
+      <c r="A23" s="307">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B23" s="319">
+      <c r="B23" s="307">
         <v>0.7055555555555556</v>
       </c>
-      <c r="D23" s="325" t="s">
+      <c r="D23" s="313" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="325" t="s">
+      <c r="E23" s="313" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="319"/>
-      <c r="B24" s="319"/>
+      <c r="A24" s="307"/>
+      <c r="B24" s="307"/>
       <c r="E24">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="318" t="s">
+      <c r="A25" s="306" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="294" t="s">
+      <c r="D25" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="294"/>
+      <c r="E25" s="338"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="316">
+      <c r="A26" s="304">
         <v>43841</v>
       </c>
-      <c r="B26" s="320"/>
+      <c r="B26" s="308"/>
       <c r="C26" s="282"/>
       <c r="D26" s="282"/>
       <c r="E26" s="282"/>
       <c r="F26" s="282"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="317" t="s">
+      <c r="A27" s="305" t="s">
         <v>192</v>
       </c>
-      <c r="B27" s="317" t="s">
+      <c r="B27" s="305" t="s">
         <v>205</v>
       </c>
-      <c r="D27" s="326" t="s">
+      <c r="D27" s="314" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="326" t="s">
+      <c r="E27" s="314" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="317" t="s">
+      <c r="A28" s="305" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="317" t="s">
+      <c r="B28" s="305" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="326" t="s">
+      <c r="D28" s="314" t="s">
         <v>223</v>
       </c>
-      <c r="E28" s="326" t="s">
+      <c r="E28" s="314" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="317" t="s">
+      <c r="A29" s="305" t="s">
         <v>208</v>
       </c>
-      <c r="B29" s="317" t="s">
+      <c r="B29" s="305" t="s">
         <v>209</v>
       </c>
-      <c r="D29" s="326" t="s">
+      <c r="D29" s="314" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="326" t="s">
+      <c r="E29" s="314" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="317" t="s">
+      <c r="A30" s="305" t="s">
         <v>201</v>
       </c>
-      <c r="B30" s="317" t="s">
+      <c r="B30" s="305" t="s">
         <v>210</v>
       </c>
-      <c r="D30" s="326" t="s">
+      <c r="D30" s="314" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="326" t="s">
+      <c r="E30" s="314" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="317" t="s">
+      <c r="A31" s="305" t="s">
         <v>211</v>
       </c>
-      <c r="B31" s="317" t="s">
+      <c r="B31" s="305" t="s">
         <v>212</v>
       </c>
-      <c r="D31" s="326" t="s">
+      <c r="D31" s="314" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="326" t="s">
+      <c r="E31" s="314" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="317" t="s">
+      <c r="A32" s="305" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="317" t="s">
+      <c r="B32" s="305" t="s">
         <v>214</v>
       </c>
-      <c r="D32" s="327" t="s">
+      <c r="D32" s="315" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="327" t="s">
+      <c r="E32" s="315" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="317" t="s">
+      <c r="A33" s="305" t="s">
         <v>215</v>
       </c>
-      <c r="B33" s="317" t="s">
+      <c r="B33" s="305" t="s">
         <v>216</v>
       </c>
-      <c r="D33" s="327" t="s">
+      <c r="D33" s="315" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="327" t="s">
+      <c r="E33" s="315" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="317" t="s">
+      <c r="A34" s="305" t="s">
         <v>217</v>
       </c>
-      <c r="B34" s="317" t="s">
+      <c r="B34" s="305" t="s">
         <v>218</v>
       </c>
-      <c r="D34" s="327" t="s">
+      <c r="D34" s="315" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="327" t="s">
+      <c r="E34" s="315" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="317" t="s">
+      <c r="A35" s="305" t="s">
         <v>219</v>
       </c>
-      <c r="B35" s="317" t="s">
+      <c r="B35" s="305" t="s">
         <v>220</v>
       </c>
-      <c r="D35" s="327" t="s">
+      <c r="D35" s="315" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="327" t="s">
+      <c r="E35" s="315" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="317" t="s">
+      <c r="A36" s="305" t="s">
         <v>221</v>
       </c>
-      <c r="B36" s="317" t="s">
+      <c r="B36" s="305" t="s">
         <v>222</v>
       </c>
-      <c r="D36" s="327" t="s">
+      <c r="D36" s="315" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="327" t="s">
+      <c r="E36" s="315" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="319">
+      <c r="A37" s="307">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B37" s="319">
+      <c r="B37" s="307">
         <v>0.55555555555555558</v>
       </c>
-      <c r="D37" s="328" t="s">
+      <c r="D37" s="316" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="328" t="s">
+      <c r="E37" s="316" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="319">
+      <c r="A38" s="307">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B38" s="319">
+      <c r="B38" s="307">
         <v>0.57222222222222219</v>
       </c>
-      <c r="D38" s="328" t="s">
+      <c r="D38" s="316" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="328" t="s">
+      <c r="E38" s="316" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="319">
+      <c r="A39" s="307">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B39" s="319">
+      <c r="B39" s="307">
         <v>0.58888888888888891</v>
       </c>
-      <c r="D39" s="328" t="s">
+      <c r="D39" s="316" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="328" t="s">
+      <c r="E39" s="316" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="319">
+      <c r="A40" s="307">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B40" s="319">
+      <c r="B40" s="307">
         <v>0.60555555555555551</v>
       </c>
-      <c r="D40" s="328" t="s">
+      <c r="D40" s="316" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="328" t="s">
+      <c r="E40" s="316" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="319">
+      <c r="A41" s="307">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B41" s="319">
+      <c r="B41" s="307">
         <v>0.62222222222222223</v>
       </c>
-      <c r="D41" s="328" t="s">
+      <c r="D41" s="316" t="s">
         <v>156</v>
       </c>
-      <c r="E41" s="328" t="s">
+      <c r="E41" s="316" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="319"/>
-      <c r="B42" s="319"/>
+      <c r="A42" s="307"/>
+      <c r="B42" s="307"/>
       <c r="E42">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="318" t="s">
+      <c r="A43" s="306" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="294" t="s">
+      <c r="D43" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="E43" s="294"/>
+      <c r="E43" s="338"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="316">
+      <c r="A44" s="304">
         <v>43848</v>
       </c>
-      <c r="B44" s="320"/>
+      <c r="B44" s="308"/>
       <c r="C44" s="282"/>
       <c r="D44" s="282"/>
       <c r="E44" s="282"/>
       <c r="F44" s="282"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="317" t="s">
+      <c r="A45" s="305" t="s">
         <v>192</v>
       </c>
-      <c r="B45" s="317" t="s">
+      <c r="B45" s="305" t="s">
         <v>205</v>
       </c>
       <c r="C45" s="9"/>
-      <c r="D45" s="329" t="s">
+      <c r="D45" s="317" t="s">
         <v>102</v>
       </c>
-      <c r="E45" s="329" t="s">
+      <c r="E45" s="317" t="s">
         <v>107</v>
       </c>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="317" t="s">
+      <c r="A46" s="305" t="s">
         <v>206</v>
       </c>
-      <c r="B46" s="317" t="s">
+      <c r="B46" s="305" t="s">
         <v>207</v>
       </c>
       <c r="C46" s="9"/>
-      <c r="D46" s="329" t="s">
+      <c r="D46" s="317" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="329" t="s">
+      <c r="E46" s="317" t="s">
         <v>102</v>
       </c>
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="317" t="s">
+      <c r="A47" s="305" t="s">
         <v>208</v>
       </c>
-      <c r="B47" s="317" t="s">
+      <c r="B47" s="305" t="s">
         <v>209</v>
       </c>
       <c r="C47" s="9"/>
-      <c r="D47" s="329" t="s">
+      <c r="D47" s="317" t="s">
         <v>107</v>
       </c>
-      <c r="E47" s="329" t="s">
+      <c r="E47" s="317" t="s">
         <v>163</v>
       </c>
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="317" t="s">
+      <c r="A48" s="305" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="317" t="s">
+      <c r="B48" s="305" t="s">
         <v>210</v>
       </c>
       <c r="C48" s="9"/>
-      <c r="D48" s="329" t="s">
+      <c r="D48" s="317" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="329" t="s">
+      <c r="E48" s="317" t="s">
         <v>163</v>
       </c>
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="317" t="s">
+      <c r="A49" s="305" t="s">
         <v>211</v>
       </c>
-      <c r="B49" s="317" t="s">
+      <c r="B49" s="305" t="s">
         <v>212</v>
       </c>
       <c r="C49" s="9"/>
-      <c r="D49" s="324" t="s">
+      <c r="D49" s="312" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="324" t="s">
+      <c r="E49" s="312" t="s">
         <v>76</v>
       </c>
       <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="317" t="s">
+      <c r="A50" s="305" t="s">
         <v>213</v>
       </c>
-      <c r="B50" s="317" t="s">
+      <c r="B50" s="305" t="s">
         <v>214</v>
       </c>
       <c r="C50" s="9"/>
-      <c r="D50" s="324" t="s">
+      <c r="D50" s="312" t="s">
         <v>77</v>
       </c>
-      <c r="E50" s="324" t="s">
+      <c r="E50" s="312" t="s">
         <v>76</v>
       </c>
       <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="317" t="s">
+      <c r="A51" s="305" t="s">
         <v>215</v>
       </c>
-      <c r="B51" s="317" t="s">
+      <c r="B51" s="305" t="s">
         <v>216</v>
       </c>
       <c r="C51" s="9"/>
-      <c r="D51" s="324" t="s">
+      <c r="D51" s="312" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="324" t="s">
+      <c r="E51" s="312" t="s">
         <v>74</v>
       </c>
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="317" t="s">
+      <c r="A52" s="305" t="s">
         <v>217</v>
       </c>
-      <c r="B52" s="317" t="s">
+      <c r="B52" s="305" t="s">
         <v>218</v>
       </c>
       <c r="C52" s="9"/>
-      <c r="D52" s="324" t="s">
+      <c r="D52" s="312" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="324" t="s">
+      <c r="E52" s="312" t="s">
         <v>74</v>
       </c>
       <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="317" t="s">
+      <c r="A53" s="305" t="s">
         <v>219</v>
       </c>
-      <c r="B53" s="317" t="s">
+      <c r="B53" s="305" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="9"/>
-      <c r="D53" s="330" t="s">
+      <c r="D53" s="318" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="330" t="s">
+      <c r="E53" s="318" t="s">
         <v>62</v>
       </c>
       <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="317" t="s">
+      <c r="A54" s="305" t="s">
         <v>221</v>
       </c>
-      <c r="B54" s="317" t="s">
+      <c r="B54" s="305" t="s">
         <v>222</v>
       </c>
       <c r="C54" s="9"/>
-      <c r="D54" s="330" t="s">
+      <c r="D54" s="318" t="s">
         <v>62</v>
       </c>
-      <c r="E54" s="330" t="s">
+      <c r="E54" s="318" t="s">
         <v>58</v>
       </c>
       <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="319">
+      <c r="A55" s="307">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B55" s="319">
+      <c r="B55" s="307">
         <v>0.55555555555555558</v>
       </c>
       <c r="C55" s="9"/>
-      <c r="D55" s="330" t="s">
+      <c r="D55" s="318" t="s">
         <v>61</v>
       </c>
-      <c r="E55" s="330" t="s">
+      <c r="E55" s="318" t="s">
         <v>59</v>
       </c>
       <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="319">
+      <c r="A56" s="307">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B56" s="319">
+      <c r="B56" s="307">
         <v>0.57222222222222219</v>
       </c>
       <c r="C56" s="9"/>
-      <c r="D56" s="331" t="s">
+      <c r="D56" s="319" t="s">
         <v>58</v>
       </c>
-      <c r="E56" s="331" t="s">
+      <c r="E56" s="319" t="s">
         <v>60</v>
       </c>
       <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="319">
+      <c r="A57" s="307">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B57" s="319">
+      <c r="B57" s="307">
         <v>0.58888888888888891</v>
       </c>
       <c r="C57" s="9"/>
-      <c r="D57" s="331" t="s">
+      <c r="D57" s="319" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="331" t="s">
+      <c r="E57" s="319" t="s">
         <v>61</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="319"/>
-      <c r="B58" s="319"/>
+      <c r="A58" s="307"/>
+      <c r="B58" s="307"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9">
@@ -26182,86 +26190,86 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="333" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="332"/>
+    <col min="1" max="1" width="26.33203125" style="321" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="320"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="335" t="s">
+      <c r="A2" s="323" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="334">
+      <c r="B2" s="322">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="335" t="s">
+      <c r="A3" s="323" t="s">
         <v>233</v>
       </c>
-      <c r="B3" s="334"/>
+      <c r="B3" s="322"/>
     </row>
     <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="335" t="s">
+      <c r="A4" s="323" t="s">
         <v>232</v>
       </c>
-      <c r="B4" s="334"/>
+      <c r="B4" s="322"/>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="335" t="s">
+      <c r="A5" s="323" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="334"/>
+      <c r="B5" s="322"/>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="335" t="s">
+      <c r="A6" s="323" t="s">
         <v>230</v>
       </c>
-      <c r="B6" s="334"/>
+      <c r="B6" s="322"/>
     </row>
     <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="335" t="s">
+      <c r="A7" s="323" t="s">
         <v>229</v>
       </c>
-      <c r="B7" s="334">
+      <c r="B7" s="322">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="335" t="s">
+      <c r="A8" s="323" t="s">
         <v>228</v>
       </c>
-      <c r="B8" s="334"/>
+      <c r="B8" s="322"/>
     </row>
     <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="335" t="s">
+      <c r="A9" s="323" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="334"/>
+      <c r="B9" s="322"/>
     </row>
     <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="335" t="s">
+      <c r="A10" s="323" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="334"/>
+      <c r="B10" s="322"/>
     </row>
     <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="335" t="s">
+      <c r="A11" s="323" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="334"/>
+      <c r="B11" s="322"/>
     </row>
     <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="335" t="s">
+      <c r="A12" s="323" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="334">
+      <c r="B12" s="322">
         <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="332">
+      <c r="B14" s="320">
         <f>SUM(B2:B13)</f>
         <v>243</v>
       </c>

</xml_diff>